<commit_message>
added management interface to mx common
</commit_message>
<xml_diff>
--- a/vmx_test_lab.xlsx
+++ b/vmx_test_lab.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aburston\Documents\src\foghorn\vmx-test-lab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B21170C-2161-42A8-869B-D80D31910245}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7D0AEF4-F9EF-4D47-8F20-12C0B9336DE6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="base" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="178">
   <si>
     <t>host</t>
   </si>
@@ -55,9 +55,6 @@
     <t>OS_version</t>
   </si>
   <si>
-    <t>20.1R1.11</t>
-  </si>
-  <si>
     <t>autonomous_system</t>
   </si>
   <si>
@@ -388,12 +385,6 @@
     <t>ge-0/0/4</t>
   </si>
   <si>
-    <t>10.1.1.1</t>
-  </si>
-  <si>
-    <t>10.1.1.5</t>
-  </si>
-  <si>
     <t>10.2.1.5</t>
   </si>
   <si>
@@ -409,45 +400,12 @@
     <t>*** to bos-2 ***</t>
   </si>
   <si>
-    <t>10.1.1.9</t>
-  </si>
-  <si>
-    <t>10.1.1.13</t>
-  </si>
-  <si>
-    <t>10.1.2.1</t>
-  </si>
-  <si>
-    <t>10.1.2.5</t>
-  </si>
-  <si>
-    <t>10.1.2.9</t>
-  </si>
-  <si>
-    <t>10.1.2.13</t>
-  </si>
-  <si>
-    <t>*** to ce-1 ***</t>
-  </si>
-  <si>
-    <t>*** to ce-2 ***</t>
-  </si>
-  <si>
-    <t>*** to ce-3 ***</t>
-  </si>
-  <si>
-    <t>*** to ce-4 ***</t>
-  </si>
-  <si>
     <t>*** to p-1 ***</t>
   </si>
   <si>
     <t>*** to p-2 ***</t>
   </si>
   <si>
-    <t>10.1.1.2</t>
-  </si>
-  <si>
     <t>10.2.1.2</t>
   </si>
   <si>
@@ -457,9 +415,6 @@
     <t>10.4.1.2</t>
   </si>
   <si>
-    <t>10.1.2.2</t>
-  </si>
-  <si>
     <t>10.3.1.1</t>
   </si>
   <si>
@@ -472,24 +427,12 @@
     <t>*** to p-3 ***</t>
   </si>
   <si>
-    <t>10.1.1.6</t>
-  </si>
-  <si>
-    <t>10.1.2.6</t>
-  </si>
-  <si>
     <t>10.2.2.1</t>
   </si>
   <si>
     <t>10.2.2.5</t>
   </si>
   <si>
-    <t>10.1.1.10</t>
-  </si>
-  <si>
-    <t>10.1.2.10</t>
-  </si>
-  <si>
     <t>10.2.3.1</t>
   </si>
   <si>
@@ -499,12 +442,6 @@
     <t>*** to p-4 ***</t>
   </si>
   <si>
-    <t>10.1.1.14</t>
-  </si>
-  <si>
-    <t>10.1.2.14</t>
-  </si>
-  <si>
     <t>10.2.4.1</t>
   </si>
   <si>
@@ -562,9 +499,6 @@
     <t>10.3.2.2</t>
   </si>
   <si>
-    <t>10.5.2.2</t>
-  </si>
-  <si>
     <t>10.3.2.6</t>
   </si>
   <si>
@@ -583,34 +517,49 @@
     <t>*** to pe-4 ***</t>
   </si>
   <si>
-    <t>10.5.1.1</t>
-  </si>
-  <si>
-    <t>10.5.1.5</t>
-  </si>
-  <si>
     <t>10.3.2.10</t>
   </si>
   <si>
-    <t>10.5.1.2</t>
-  </si>
-  <si>
     <t>10.4.2.2</t>
   </si>
   <si>
-    <t>10.5.2.1</t>
-  </si>
-  <si>
-    <t>10.5.2.5</t>
-  </si>
-  <si>
     <t>10.4.2.6</t>
   </si>
   <si>
-    <t>10.5.1.6</t>
-  </si>
-  <si>
-    <t>10.5.2.6</t>
+    <t>20.2R1.10</t>
+  </si>
+  <si>
+    <t>iso_address</t>
+  </si>
+  <si>
+    <t>47.0005.80ff.f800.0000.0108.0001.0100.5210.0004.00</t>
+  </si>
+  <si>
+    <t>47.0005.80ff.f800.0000.0108.0001.0100.5210.0005.00</t>
+  </si>
+  <si>
+    <t>47.0005.80ff.f800.0000.0108.0001.0100.5210.0006.00</t>
+  </si>
+  <si>
+    <t>47.0005.80ff.f800.0000.0108.0001.0100.5210.0007.00</t>
+  </si>
+  <si>
+    <t>47.0005.80ff.f800.0000.0108.0001.0100.5210.0008.00</t>
+  </si>
+  <si>
+    <t>47.0005.80ff.f800.0000.0108.0001.0100.5210.0009.00</t>
+  </si>
+  <si>
+    <t>47.0005.80ff.f800.0000.0108.0001.0100.5210.0010.00</t>
+  </si>
+  <si>
+    <t>47.0005.80ff.f800.0000.0108.0001.0100.5210.0011.00</t>
+  </si>
+  <si>
+    <t>47.0005.80ff.f800.0000.0108.0001.0100.5210.0012.00</t>
+  </si>
+  <si>
+    <t>47.0005.80ff.f800.0000.0108.0001.0100.5210.0003.00</t>
   </si>
 </sst>
 </file>
@@ -995,10 +944,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C40"/>
+  <dimension ref="A1:C50"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1049,7 +998,7 @@
         <v>8</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>9</v>
+        <v>166</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -1057,7 +1006,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C5" s="2">
         <v>65200</v>
@@ -1068,10 +1017,10 @@
         <v>3</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -1079,10 +1028,10 @@
         <v>3</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -1090,10 +1039,10 @@
         <v>3</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -1101,10 +1050,10 @@
         <v>3</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -1112,10 +1061,10 @@
         <v>3</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -1123,10 +1072,10 @@
         <v>3</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="153.75">
@@ -1134,10 +1083,10 @@
         <v>3</v>
       </c>
       <c r="B12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -1145,10 +1094,10 @@
         <v>3</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -1156,10 +1105,10 @@
         <v>3</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -1167,10 +1116,10 @@
         <v>3</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -1178,7 +1127,7 @@
         <v>3</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C16" s="2">
         <v>22</v>
@@ -1189,10 +1138,10 @@
         <v>3</v>
       </c>
       <c r="B17" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -1200,10 +1149,10 @@
         <v>3</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -1211,10 +1160,10 @@
         <v>3</v>
       </c>
       <c r="B19" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -1222,10 +1171,10 @@
         <v>3</v>
       </c>
       <c r="B20" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -1233,10 +1182,10 @@
         <v>3</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -1244,10 +1193,10 @@
         <v>3</v>
       </c>
       <c r="B22" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -1255,7 +1204,7 @@
         <v>3</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C23" s="2">
         <v>800</v>
@@ -1266,10 +1215,10 @@
         <v>3</v>
       </c>
       <c r="B24" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -1277,131 +1226,131 @@
         <v>3</v>
       </c>
       <c r="B25" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C25" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B26" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="27" spans="1:3">
       <c r="A27" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="28" spans="1:3">
       <c r="A28" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="29" spans="1:3">
       <c r="A29" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>46</v>
+        <v>167</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>93</v>
+        <v>177</v>
       </c>
     </row>
     <row r="30" spans="1:3">
       <c r="A30" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="31" spans="1:3">
       <c r="A31" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>46</v>
+        <v>167</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>95</v>
+        <v>168</v>
       </c>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="2" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="2" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>46</v>
+        <v>167</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>97</v>
+        <v>169</v>
       </c>
     </row>
     <row r="34" spans="1:3">
       <c r="A34" s="2" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="2" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>46</v>
+        <v>167</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>99</v>
+        <v>170</v>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -1409,43 +1358,153 @@
         <v>87</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>46</v>
+        <v>167</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>101</v>
+        <v>171</v>
       </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" s="2" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="39" spans="1:3">
       <c r="A39" s="2" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>46</v>
+        <v>167</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>103</v>
+        <v>172</v>
       </c>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" s="2" t="s">
-        <v>49</v>
+        <v>89</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>32</v>
+        <v>97</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -1475,10 +1534,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -1486,10 +1545,10 @@
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>52</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1518,10 +1577,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -1529,10 +1588,10 @@
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1563,13 +1622,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1577,13 +1636,13 @@
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>61</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1600,7 +1659,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1614,24 +1673,24 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>67</v>
       </c>
       <c r="D2" s="2">
         <v>16</v>
@@ -1639,13 +1698,13 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D3" s="2">
         <v>16</v>
@@ -1653,13 +1712,13 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D4" s="2">
         <v>16</v>
@@ -1667,13 +1726,13 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D5" s="2">
         <v>16</v>
@@ -1681,13 +1740,13 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D6" s="2">
         <v>16</v>
@@ -1695,13 +1754,13 @@
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D7" s="2">
         <v>16</v>
@@ -1709,13 +1768,13 @@
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D8" s="2">
         <v>16</v>
@@ -1723,13 +1782,13 @@
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D9" s="2">
         <v>16</v>
@@ -1737,13 +1796,13 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D10" s="2">
         <v>16</v>
@@ -1751,13 +1810,13 @@
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D11" s="2">
         <v>16</v>
@@ -1765,13 +1824,13 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D12" s="2">
         <v>16</v>
@@ -1779,13 +1838,13 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D13" s="2">
         <v>16</v>
@@ -1793,13 +1852,13 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D14" s="2">
         <v>16</v>
@@ -1807,13 +1866,13 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D15" s="2">
         <v>16</v>
@@ -1821,13 +1880,13 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B16" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>69</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>70</v>
       </c>
       <c r="D16" s="2">
         <v>16</v>
@@ -1845,10 +1904,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:E59"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A62" sqref="A62"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1863,30 +1922,30 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>73</v>
+        <v>117</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="E2" s="2">
         <v>30</v>
@@ -1894,16 +1953,16 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="2" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>72</v>
+        <v>118</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E3" s="2">
         <v>30</v>
@@ -1911,16 +1970,16 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="2" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="E4" s="2">
         <v>30</v>
@@ -1928,16 +1987,16 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="2" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c r="E5" s="2">
         <v>30</v>
@@ -1945,16 +2004,16 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>73</v>
+        <v>117</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>129</v>
+        <v>135</v>
       </c>
       <c r="E6" s="2">
         <v>30</v>
@@ -1962,16 +2021,16 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>72</v>
+        <v>118</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="E7" s="2">
         <v>30</v>
@@ -1979,16 +2038,16 @@
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="2" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
       <c r="E8" s="2">
         <v>30</v>
@@ -1996,16 +2055,16 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="2" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="E9" s="2">
         <v>30</v>
@@ -2013,16 +2072,16 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="2" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>133</v>
+        <v>115</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
       <c r="E10" s="2">
         <v>30</v>
@@ -2030,16 +2089,16 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="2" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>134</v>
+        <v>116</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="E11" s="2">
         <v>30</v>
@@ -2047,16 +2106,16 @@
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="2" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>137</v>
+        <v>122</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E12" s="2">
         <v>30</v>
@@ -2064,16 +2123,16 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="2" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>138</v>
+        <v>123</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>122</v>
+        <v>147</v>
       </c>
       <c r="E13" s="2">
         <v>30</v>
@@ -2081,16 +2140,16 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="2" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>73</v>
+        <v>140</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>148</v>
+        <v>129</v>
       </c>
       <c r="E14" s="2">
         <v>30</v>
@@ -2098,16 +2157,16 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="2" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>72</v>
+        <v>141</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>149</v>
+        <v>120</v>
       </c>
       <c r="E15" s="2">
         <v>30</v>
@@ -2115,16 +2174,16 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="2" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>118</v>
+        <v>72</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="E16" s="2">
         <v>30</v>
@@ -2132,16 +2191,16 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="2" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>147</v>
+        <v>122</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>119</v>
+        <v>71</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="E17" s="2">
         <v>30</v>
@@ -2149,16 +2208,16 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="2" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>73</v>
+        <v>117</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="E18" s="2">
         <v>30</v>
@@ -2166,16 +2225,16 @@
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="2" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>72</v>
+        <v>118</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="E19" s="2">
         <v>30</v>
@@ -2183,16 +2242,16 @@
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="2" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>137</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>118</v>
+        <v>140</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="E20" s="2">
         <v>30</v>
@@ -2200,16 +2259,16 @@
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="2" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>119</v>
+        <v>141</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="E21" s="2">
         <v>30</v>
@@ -2217,16 +2276,16 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="2" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>133</v>
+        <v>116</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="E22" s="2">
         <v>30</v>
@@ -2234,16 +2293,16 @@
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="2" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>158</v>
+        <v>127</v>
       </c>
       <c r="E23" s="2">
         <v>30</v>
@@ -2251,16 +2310,16 @@
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="2" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="E24" s="2">
         <v>30</v>
@@ -2268,16 +2327,16 @@
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="2" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="E25" s="2">
         <v>30</v>
@@ -2285,16 +2344,16 @@
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>116</v>
+        <v>153</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>73</v>
+        <v>140</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>140</v>
+        <v>121</v>
       </c>
       <c r="E26" s="2">
         <v>30</v>
@@ -2302,16 +2361,16 @@
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="2" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>72</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E27" s="2">
         <v>30</v>
@@ -2319,16 +2378,16 @@
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="2" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>125</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>118</v>
+        <v>71</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="E28" s="2">
         <v>30</v>
@@ -2336,16 +2395,16 @@
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="2" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>126</v>
+        <v>143</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="E29" s="2">
         <v>30</v>
@@ -2353,16 +2412,16 @@
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="2" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>161</v>
+        <v>118</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>144</v>
+        <v>159</v>
       </c>
       <c r="E30" s="2">
         <v>30</v>
@@ -2370,16 +2429,16 @@
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>162</v>
+        <v>117</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>123</v>
+        <v>163</v>
       </c>
       <c r="E31" s="2">
         <v>30</v>
@@ -2387,16 +2446,16 @@
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="2" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>116</v>
+        <v>161</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>73</v>
+        <v>118</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>165</v>
+        <v>128</v>
       </c>
       <c r="E32" s="2">
         <v>30</v>
@@ -2404,16 +2463,16 @@
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="2" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>125</v>
+        <v>162</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>72</v>
+        <v>140</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="E33" s="2">
         <v>30</v>
@@ -2421,16 +2480,16 @@
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>126</v>
+        <v>161</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>170</v>
+        <v>146</v>
       </c>
       <c r="E34" s="2">
         <v>30</v>
@@ -2438,426 +2497,18 @@
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>147</v>
+        <v>162</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="E35" s="2">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5">
-      <c r="A36" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="E36" s="2">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5">
-      <c r="A37" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="E37" s="2">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5">
-      <c r="A38" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E38" s="2">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5">
-      <c r="A39" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="E39" s="2">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5">
-      <c r="A40" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="E40" s="2">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5">
-      <c r="A41" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="E41" s="2">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5">
-      <c r="A42" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="E42" s="2">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5">
-      <c r="A43" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="E43" s="2">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5">
-      <c r="A44" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="E44" s="2">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5">
-      <c r="A45" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="E45" s="2">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5">
-      <c r="A46" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="E46" s="2">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5">
-      <c r="A47" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B47" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="E47" s="2">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5">
-      <c r="A48" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B48" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>186</v>
-      </c>
-      <c r="E48" s="2">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5">
-      <c r="A49" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="E49" s="2">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5">
-      <c r="A50" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B50" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="D50" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="E50" s="2">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5">
-      <c r="A51" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="E51" s="2">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5">
-      <c r="A52" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="D52" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="E52" s="2">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5">
-      <c r="A53" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D53" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="E53" s="2">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5">
-      <c r="A54" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="D54" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="E54" s="2">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5">
-      <c r="A55" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="B55" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>192</v>
-      </c>
-      <c r="E55" s="2">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5">
-      <c r="A56" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="D56" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="E56" s="2">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5">
-      <c r="A57" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D57" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="E57" s="2">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5">
-      <c r="A58" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="D58" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="E58" s="2">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5">
-      <c r="A59" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B59" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D59" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="E59" s="2">
         <v>30</v>
       </c>
     </row>
@@ -2873,10 +2524,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:E59"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="E53" sqref="E53"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2893,1002 +2544,594 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="B2" s="2">
-        <v>65400</v>
+        <v>65402</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D2" s="2">
-        <v>65402</v>
+        <v>65406</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="2" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="B3" s="2">
-        <v>65400</v>
+        <v>65402</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D3" s="2">
-        <v>65403</v>
+        <v>65407</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="2" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="B4" s="2">
-        <v>65400</v>
+        <v>65403</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D4" s="2">
-        <v>65404</v>
+        <v>65406</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>152</v>
+        <v>131</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="2" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="B5" s="2">
-        <v>65400</v>
+        <v>65403</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D5" s="2">
-        <v>65405</v>
+        <v>65408</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B6" s="2">
-        <v>65401</v>
+        <v>65404</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D6" s="2">
-        <v>65402</v>
+        <v>65406</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B7" s="2">
-        <v>65401</v>
+        <v>65404</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D7" s="2">
-        <v>65403</v>
+        <v>65407</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="2" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="B8" s="2">
-        <v>65401</v>
+        <v>65405</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D8" s="2">
-        <v>65404</v>
+        <v>65406</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="2" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="B9" s="2">
-        <v>65401</v>
+        <v>65405</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D9" s="2">
-        <v>65405</v>
+        <v>65407</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="2" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="B10" s="2">
+        <v>65406</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D10" s="2">
         <v>65402</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="D10" s="2">
-        <v>65400</v>
-      </c>
       <c r="E10" s="2" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="2" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="B11" s="2">
-        <v>65402</v>
+        <v>65406</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D11" s="2">
-        <v>65401</v>
+        <v>65403</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="2" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="B12" s="2">
-        <v>65402</v>
+        <v>65406</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D12" s="2">
-        <v>65406</v>
+        <v>65404</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="2" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="B13" s="2">
-        <v>65402</v>
+        <v>65406</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D13" s="2">
-        <v>65407</v>
+        <v>65405</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>165</v>
+        <v>138</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="2" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B14" s="2">
-        <v>65403</v>
+        <v>65406</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D14" s="2">
-        <v>65400</v>
+        <v>65408</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="2" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B15" s="2">
-        <v>65403</v>
+        <v>65406</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D15" s="2">
-        <v>65401</v>
+        <v>65409</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>130</v>
+        <v>145</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="2" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="B16" s="2">
-        <v>65403</v>
+        <v>65407</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D16" s="2">
-        <v>65406</v>
+        <v>65402</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>146</v>
+        <v>119</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="2" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="B17" s="2">
-        <v>65403</v>
+        <v>65407</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D17" s="2">
-        <v>65408</v>
+        <v>65404</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>175</v>
+        <v>136</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="2" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="B18" s="2">
-        <v>65404</v>
+        <v>65407</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D18" s="2">
-        <v>65400</v>
+        <v>65405</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>127</v>
+        <v>139</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="2" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="B19" s="2">
-        <v>65404</v>
+        <v>65407</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D19" s="2">
-        <v>65401</v>
+        <v>65408</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>131</v>
+        <v>156</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="2" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="B20" s="2">
-        <v>65404</v>
+        <v>65407</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D20" s="2">
-        <v>65406</v>
+        <v>65409</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="2" t="s">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="B21" s="2">
-        <v>65404</v>
+        <v>65407</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D21" s="2">
-        <v>65407</v>
+        <v>65410</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="2" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="B22" s="2">
-        <v>65405</v>
+        <v>65408</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D22" s="2">
-        <v>65400</v>
+        <v>65403</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>128</v>
+        <v>134</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="2" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="B23" s="2">
-        <v>65405</v>
+        <v>65408</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D23" s="2">
-        <v>65401</v>
+        <v>65406</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="2" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="B24" s="2">
-        <v>65405</v>
+        <v>65408</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D24" s="2">
-        <v>65406</v>
+        <v>65407</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>168</v>
+        <v>150</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="2" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="B25" s="2">
-        <v>65405</v>
+        <v>65408</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D25" s="2">
-        <v>65407</v>
+        <v>65410</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>170</v>
+        <v>128</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B26" s="2">
-        <v>65406</v>
+        <v>65408</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D26" s="2">
-        <v>65402</v>
+        <v>65411</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="2" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B27" s="2">
+        <v>65409</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D27" s="2">
         <v>65406</v>
       </c>
-      <c r="C27" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="D27" s="2">
-        <v>65403</v>
-      </c>
       <c r="E27" s="2" t="s">
-        <v>150</v>
+        <v>120</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="2" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B28" s="2">
-        <v>65406</v>
+        <v>65409</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D28" s="2">
-        <v>65404</v>
+        <v>65407</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="2" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B29" s="2">
-        <v>65406</v>
+        <v>65409</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D29" s="2">
-        <v>65405</v>
+        <v>65410</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="2" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B30" s="2">
-        <v>65406</v>
+        <v>65409</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D30" s="2">
-        <v>65408</v>
+        <v>65411</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>141</v>
+        <v>165</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="2" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B31" s="2">
-        <v>65406</v>
+        <v>65410</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D31" s="2">
-        <v>65409</v>
+        <v>65407</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>166</v>
+        <v>152</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="2" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B32" s="2">
-        <v>65407</v>
+        <v>65410</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D32" s="2">
-        <v>65402</v>
+        <v>65408</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>122</v>
+        <v>155</v>
       </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="2" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B33" s="2">
-        <v>65407</v>
+        <v>65410</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D33" s="2">
-        <v>65404</v>
+        <v>65409</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B34" s="2">
-        <v>65407</v>
+        <v>65411</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D34" s="2">
-        <v>65405</v>
+        <v>65408</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>160</v>
+        <v>121</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="2" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B35" s="2">
-        <v>65407</v>
+        <v>65411</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D35" s="2">
-        <v>65408</v>
+        <v>65409</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5">
-      <c r="A36" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="B36" s="2">
-        <v>65407</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="D36" s="2">
-        <v>65409</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5">
-      <c r="A37" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="B37" s="2">
-        <v>65407</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="D37" s="2">
-        <v>65410</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5">
-      <c r="A38" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B38" s="2">
-        <v>65408</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="D38" s="2">
-        <v>65403</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5">
-      <c r="A39" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B39" s="2">
-        <v>65408</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="D39" s="2">
-        <v>65406</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5">
-      <c r="A40" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B40" s="2">
-        <v>65408</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="D40" s="2">
-        <v>65407</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5">
-      <c r="A41" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B41" s="2">
-        <v>65408</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="D41" s="2">
-        <v>65410</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5">
-      <c r="A42" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B42" s="2">
-        <v>65408</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="D42" s="2">
-        <v>65411</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5">
-      <c r="A43" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="B43" s="2">
-        <v>65409</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="D43" s="2">
-        <v>65406</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5">
-      <c r="A44" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="B44" s="2">
-        <v>65409</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="D44" s="2">
-        <v>65407</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5">
-      <c r="A45" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="B45" s="2">
-        <v>65409</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="D45" s="2">
-        <v>65410</v>
-      </c>
-      <c r="E45" s="2" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5">
-      <c r="A46" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="B46" s="2">
-        <v>65409</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="D46" s="2">
-        <v>65411</v>
-      </c>
-      <c r="E46" s="2" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5">
-      <c r="A47" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B47" s="2">
-        <v>65410</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="D47" s="2">
-        <v>65412</v>
-      </c>
-      <c r="E47" s="2" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5">
-      <c r="A48" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B48" s="2">
-        <v>65410</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="D48" s="2">
-        <v>65413</v>
-      </c>
-      <c r="E48" s="2" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5">
-      <c r="A49" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B49" s="2">
-        <v>65410</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="D49" s="2">
-        <v>65407</v>
-      </c>
-      <c r="E49" s="2" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5">
-      <c r="A50" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B50" s="2">
-        <v>65410</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="D50" s="2">
-        <v>65408</v>
-      </c>
-      <c r="E50" s="2" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5">
-      <c r="A51" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B51" s="2">
-        <v>65410</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="D51" s="2">
-        <v>65409</v>
-      </c>
-      <c r="E51" s="2" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5">
-      <c r="A52" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="B52" s="2">
-        <v>65411</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="D52" s="2">
-        <v>65412</v>
-      </c>
-      <c r="E52" s="2" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5">
-      <c r="A53" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="B53" s="2">
-        <v>65411</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="D53" s="2">
-        <v>65413</v>
-      </c>
-      <c r="E53" s="2" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5">
-      <c r="A54" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="B54" s="2">
-        <v>65411</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="D54" s="2">
-        <v>65408</v>
-      </c>
-      <c r="E54" s="2" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5">
-      <c r="A55" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="B55" s="2">
-        <v>65411</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="D55" s="2">
-        <v>65409</v>
-      </c>
-      <c r="E55" s="2" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5">
-      <c r="A56" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="B56" s="2">
-        <v>65412</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="D56" s="2">
-        <v>65410</v>
-      </c>
-      <c r="E56" s="2" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5">
-      <c r="A57" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="B57" s="2">
-        <v>65412</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="D57" s="2">
-        <v>65411</v>
-      </c>
-      <c r="E57" s="2" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5">
-      <c r="A58" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B58" s="2">
-        <v>65413</v>
-      </c>
-      <c r="C58" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="D58" s="2">
-        <v>65410</v>
-      </c>
-      <c r="E58" s="2" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5">
-      <c r="A59" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B59" s="2">
-        <v>65413</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="D59" s="2">
-        <v>65411</v>
-      </c>
-      <c r="E59" s="2" t="s">
-        <v>191</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
first cut at adding ibgp mesh betwwen pes
</commit_message>
<xml_diff>
--- a/vmx_test_lab.xlsx
+++ b/vmx_test_lab.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aburston\Documents\src\foghorn\vmx-test-lab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3D91560-56D1-406D-B9B8-1ED77DD31FD6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAD0973F-D906-496E-901D-B35CE634EF71}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="base" sheetId="1" r:id="rId1"/>
@@ -19,13 +19,14 @@
     <sheet name="snmp" sheetId="4" r:id="rId4"/>
     <sheet name="management_interface" sheetId="5" r:id="rId5"/>
     <sheet name="core_interfaces+" sheetId="6" r:id="rId6"/>
+    <sheet name="vpn_ibgp+" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="177">
   <si>
     <t>host</t>
   </si>
@@ -547,6 +548,15 @@
   </si>
   <si>
     <t>47.0005.80ff.f800.0000.0108.0001.0100.5210.0003.00</t>
+  </si>
+  <si>
+    <t>@group</t>
+  </si>
+  <si>
+    <t>neighbors+.name</t>
+  </si>
+  <si>
+    <t>VPN_iBGP</t>
   </si>
 </sst>
 </file>
@@ -621,10 +631,13 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="2"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1893,7 +1906,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
@@ -2507,4 +2520,369 @@
     <oddFooter>&amp;C&amp;1#&amp;"Calibri"&amp;7&amp;K000000Juniper Business Use Only</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{900D9312-7827-4356-85DE-19A6CD36A09C}">
+  <dimension ref="A1:C31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="27.5703125" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;1#&amp;"Calibri"&amp;7&amp;K000000Juniper Business Use Only</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
changed data to match new lab
</commit_message>
<xml_diff>
--- a/vmx_test_lab.xlsx
+++ b/vmx_test_lab.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aburston\Documents\src\foghorn\vmx-test-lab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAD0973F-D906-496E-901D-B35CE634EF71}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45C91130-C3C0-4FE3-8E6A-DCD7EF33F03A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="base" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="181">
   <si>
     <t>host</t>
   </si>
@@ -331,36 +331,6 @@
     <t>100.123.1.3</t>
   </si>
   <si>
-    <t>100.123.1.4</t>
-  </si>
-  <si>
-    <t>100.123.1.5</t>
-  </si>
-  <si>
-    <t>100.123.1.6</t>
-  </si>
-  <si>
-    <t>100.123.1.7</t>
-  </si>
-  <si>
-    <t>100.123.1.8</t>
-  </si>
-  <si>
-    <t>100.123.1.9</t>
-  </si>
-  <si>
-    <t>100.123.1.10</t>
-  </si>
-  <si>
-    <t>100.123.1.11</t>
-  </si>
-  <si>
-    <t>100.123.1.12</t>
-  </si>
-  <si>
-    <t>100.123.1.13</t>
-  </si>
-  <si>
     <t>*** to nyc-1 ***</t>
   </si>
   <si>
@@ -557,6 +527,48 @@
   </si>
   <si>
     <t>VPN_iBGP</t>
+  </si>
+  <si>
+    <t>host_vars/ce-5.yaml</t>
+  </si>
+  <si>
+    <t>host_vars/ce-6.yaml</t>
+  </si>
+  <si>
+    <t>100.123.28.1</t>
+  </si>
+  <si>
+    <t>100.123.28.2</t>
+  </si>
+  <si>
+    <t>100.123.28.3</t>
+  </si>
+  <si>
+    <t>100.123.28.4</t>
+  </si>
+  <si>
+    <t>100.123.28.5</t>
+  </si>
+  <si>
+    <t>100.123.28.6</t>
+  </si>
+  <si>
+    <t>100.123.28.9</t>
+  </si>
+  <si>
+    <t>100.123.28.10</t>
+  </si>
+  <si>
+    <t>100.123.28.11</t>
+  </si>
+  <si>
+    <t>100.123.28.12</t>
+  </si>
+  <si>
+    <t>100.123.28.7</t>
+  </si>
+  <si>
+    <t>100.123.28.8</t>
   </si>
 </sst>
 </file>
@@ -998,7 +1010,7 @@
         <v>8</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -1270,10 +1282,10 @@
         <v>78</v>
       </c>
       <c r="B29" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C29" s="2" t="s">
         <v>163</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -1292,10 +1304,10 @@
         <v>79</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -1314,10 +1326,10 @@
         <v>77</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -1336,10 +1348,10 @@
         <v>80</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -1358,10 +1370,10 @@
         <v>83</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -1380,10 +1392,10 @@
         <v>84</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -1402,10 +1414,10 @@
         <v>85</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -1424,10 +1436,10 @@
         <v>86</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -1446,10 +1458,10 @@
         <v>81</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -1468,10 +1480,10 @@
         <v>82</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
     </row>
     <row r="48" spans="1:3">
@@ -1656,10 +1668,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1690,7 +1702,7 @@
         <v>65</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>66</v>
+        <v>169</v>
       </c>
       <c r="D2" s="2">
         <v>16</v>
@@ -1704,7 +1716,7 @@
         <v>65</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>67</v>
+        <v>170</v>
       </c>
       <c r="D3" s="2">
         <v>16</v>
@@ -1718,7 +1730,7 @@
         <v>65</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>99</v>
+        <v>171</v>
       </c>
       <c r="D4" s="2">
         <v>16</v>
@@ -1732,7 +1744,7 @@
         <v>65</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>100</v>
+        <v>172</v>
       </c>
       <c r="D5" s="2">
         <v>16</v>
@@ -1746,7 +1758,7 @@
         <v>65</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>101</v>
+        <v>173</v>
       </c>
       <c r="D6" s="2">
         <v>16</v>
@@ -1760,7 +1772,7 @@
         <v>65</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>102</v>
+        <v>174</v>
       </c>
       <c r="D7" s="2">
         <v>16</v>
@@ -1774,7 +1786,7 @@
         <v>65</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>103</v>
+        <v>66</v>
       </c>
       <c r="D8" s="2">
         <v>16</v>
@@ -1788,7 +1800,7 @@
         <v>65</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>104</v>
+        <v>67</v>
       </c>
       <c r="D9" s="2">
         <v>16</v>
@@ -1802,7 +1814,7 @@
         <v>65</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="D10" s="2">
         <v>16</v>
@@ -1816,7 +1828,7 @@
         <v>65</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="D11" s="2">
         <v>16</v>
@@ -1830,7 +1842,7 @@
         <v>65</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>107</v>
+        <v>179</v>
       </c>
       <c r="D12" s="2">
         <v>16</v>
@@ -1844,7 +1856,7 @@
         <v>65</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>108</v>
+        <v>180</v>
       </c>
       <c r="D13" s="2">
         <v>16</v>
@@ -1858,7 +1870,7 @@
         <v>65</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>109</v>
+        <v>175</v>
       </c>
       <c r="D14" s="2">
         <v>16</v>
@@ -1872,7 +1884,7 @@
         <v>65</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>110</v>
+        <v>176</v>
       </c>
       <c r="D15" s="2">
         <v>16</v>
@@ -1880,15 +1892,43 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="D16" s="2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="D17" s="2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B18" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C18" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D18" s="2">
         <v>16</v>
       </c>
     </row>
@@ -1939,13 +1979,13 @@
         <v>78</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="E2" s="2">
         <v>30</v>
@@ -1956,13 +1996,13 @@
         <v>78</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="E3" s="2">
         <v>30</v>
@@ -1973,13 +2013,13 @@
         <v>79</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="E4" s="2">
         <v>30</v>
@@ -1990,13 +2030,13 @@
         <v>79</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="E5" s="2">
         <v>30</v>
@@ -2007,13 +2047,13 @@
         <v>77</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="E6" s="2">
         <v>30</v>
@@ -2024,13 +2064,13 @@
         <v>77</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="E7" s="2">
         <v>30</v>
@@ -2041,13 +2081,13 @@
         <v>80</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="E8" s="2">
         <v>30</v>
@@ -2058,13 +2098,13 @@
         <v>80</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="E9" s="2">
         <v>30</v>
@@ -2075,13 +2115,13 @@
         <v>83</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>72</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="E10" s="2">
         <v>30</v>
@@ -2092,13 +2132,13 @@
         <v>83</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>71</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="E11" s="2">
         <v>30</v>
@@ -2109,13 +2149,13 @@
         <v>83</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="E12" s="2">
         <v>30</v>
@@ -2126,13 +2166,13 @@
         <v>83</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="E13" s="2">
         <v>30</v>
@@ -2143,13 +2183,13 @@
         <v>83</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="E14" s="2">
         <v>30</v>
@@ -2160,13 +2200,13 @@
         <v>83</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="E15" s="2">
         <v>30</v>
@@ -2177,13 +2217,13 @@
         <v>84</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>72</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="E16" s="2">
         <v>30</v>
@@ -2194,13 +2234,13 @@
         <v>84</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>71</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="E17" s="2">
         <v>30</v>
@@ -2211,13 +2251,13 @@
         <v>84</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="E18" s="2">
         <v>30</v>
@@ -2228,13 +2268,13 @@
         <v>84</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="E19" s="2">
         <v>30</v>
@@ -2245,13 +2285,13 @@
         <v>84</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="E20" s="2">
         <v>30</v>
@@ -2262,13 +2302,13 @@
         <v>84</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="E21" s="2">
         <v>30</v>
@@ -2279,13 +2319,13 @@
         <v>85</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>72</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="E22" s="2">
         <v>30</v>
@@ -2296,13 +2336,13 @@
         <v>85</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>71</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="E23" s="2">
         <v>30</v>
@@ -2313,13 +2353,13 @@
         <v>85</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="E24" s="2">
         <v>30</v>
@@ -2330,13 +2370,13 @@
         <v>85</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="E25" s="2">
         <v>30</v>
@@ -2347,13 +2387,13 @@
         <v>85</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="E26" s="2">
         <v>30</v>
@@ -2364,13 +2404,13 @@
         <v>86</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>72</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="E27" s="2">
         <v>30</v>
@@ -2381,13 +2421,13 @@
         <v>86</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>71</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="E28" s="2">
         <v>30</v>
@@ -2398,13 +2438,13 @@
         <v>86</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="E29" s="2">
         <v>30</v>
@@ -2415,13 +2455,13 @@
         <v>86</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="E30" s="2">
         <v>30</v>
@@ -2432,13 +2472,13 @@
         <v>81</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="E31" s="2">
         <v>30</v>
@@ -2449,13 +2489,13 @@
         <v>81</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="C32" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D32" s="2" t="s">
         <v>114</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>124</v>
       </c>
       <c r="E32" s="2">
         <v>30</v>
@@ -2466,13 +2506,13 @@
         <v>81</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="E33" s="2">
         <v>30</v>
@@ -2483,13 +2523,13 @@
         <v>82</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="E34" s="2">
         <v>30</v>
@@ -2500,13 +2540,13 @@
         <v>82</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="E35" s="2">
         <v>30</v>
@@ -2526,7 +2566,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{900D9312-7827-4356-85DE-19A6CD36A09C}">
   <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
@@ -2542,10 +2582,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -2553,7 +2593,7 @@
         <v>78</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>88</v>
@@ -2564,7 +2604,7 @@
         <v>78</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>89</v>
@@ -2575,7 +2615,7 @@
         <v>78</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>90</v>
@@ -2586,7 +2626,7 @@
         <v>78</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>95</v>
@@ -2597,7 +2637,7 @@
         <v>78</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>96</v>
@@ -2608,7 +2648,7 @@
         <v>79</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>87</v>
@@ -2619,7 +2659,7 @@
         <v>79</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>89</v>
@@ -2630,7 +2670,7 @@
         <v>79</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>90</v>
@@ -2641,7 +2681,7 @@
         <v>79</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>95</v>
@@ -2652,7 +2692,7 @@
         <v>79</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>96</v>
@@ -2663,7 +2703,7 @@
         <v>77</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>87</v>
@@ -2674,7 +2714,7 @@
         <v>77</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>88</v>
@@ -2685,7 +2725,7 @@
         <v>77</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>90</v>
@@ -2696,7 +2736,7 @@
         <v>77</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>95</v>
@@ -2707,7 +2747,7 @@
         <v>77</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>96</v>
@@ -2718,7 +2758,7 @@
         <v>80</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>87</v>
@@ -2729,7 +2769,7 @@
         <v>80</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>88</v>
@@ -2740,7 +2780,7 @@
         <v>80</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>89</v>
@@ -2751,7 +2791,7 @@
         <v>80</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>95</v>
@@ -2762,7 +2802,7 @@
         <v>80</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>96</v>
@@ -2773,7 +2813,7 @@
         <v>81</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>87</v>
@@ -2784,7 +2824,7 @@
         <v>81</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>88</v>
@@ -2795,7 +2835,7 @@
         <v>81</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>89</v>
@@ -2806,7 +2846,7 @@
         <v>81</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>90</v>
@@ -2817,7 +2857,7 @@
         <v>81</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>96</v>
@@ -2828,7 +2868,7 @@
         <v>82</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>87</v>
@@ -2839,7 +2879,7 @@
         <v>82</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>88</v>
@@ -2850,7 +2890,7 @@
         <v>82</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>89</v>
@@ -2861,7 +2901,7 @@
         <v>82</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>90</v>
@@ -2872,7 +2912,7 @@
         <v>82</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>95</v>

</xml_diff>

<commit_message>
added interfaces for paragon integration
</commit_message>
<xml_diff>
--- a/vmx_test_lab.xlsx
+++ b/vmx_test_lab.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aburston\Documents\src\foghorn\vmx-test-lab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9729E1C-EC4A-47C6-813E-E7B244A151AF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A06A18A-6C21-4F12-AB3F-8287EBA958DE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="base" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="194">
   <si>
     <t>host</t>
   </si>
@@ -569,6 +569,45 @@
   </si>
   <si>
     <t>19.4R3.11</t>
+  </si>
+  <si>
+    <t>*** to k8snode1 ***</t>
+  </si>
+  <si>
+    <t>10.4.2.9</t>
+  </si>
+  <si>
+    <t>*** to k8snode2 ***</t>
+  </si>
+  <si>
+    <t>*** to k8snode3 ***</t>
+  </si>
+  <si>
+    <t>ge-0/0/7</t>
+  </si>
+  <si>
+    <t>10.4.2.13</t>
+  </si>
+  <si>
+    <t>10.4.2.17</t>
+  </si>
+  <si>
+    <t>10.4.2.10</t>
+  </si>
+  <si>
+    <t>100.123.35.1/32</t>
+  </si>
+  <si>
+    <t>100.123.35.2/32</t>
+  </si>
+  <si>
+    <t>100.123.35.3/32</t>
+  </si>
+  <si>
+    <t>10.4.2.14</t>
+  </si>
+  <si>
+    <t>10.4.2.18</t>
   </si>
 </sst>
 </file>
@@ -958,7 +997,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -1574,9 +1613,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -1604,6 +1645,39 @@
       </c>
       <c r="C2" s="2" t="s">
         <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>191</v>
       </c>
     </row>
   </sheetData>
@@ -1944,10 +2018,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:E35"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33:XFD33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2469,16 +2543,16 @@
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="2" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>146</v>
+        <v>181</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>103</v>
+        <v>126</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>149</v>
+        <v>182</v>
       </c>
       <c r="E31" s="2">
         <v>30</v>
@@ -2486,16 +2560,16 @@
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="2" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>147</v>
+        <v>183</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>104</v>
+        <v>127</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>114</v>
+        <v>186</v>
       </c>
       <c r="E32" s="2">
         <v>30</v>
@@ -2503,16 +2577,16 @@
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="2" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>148</v>
+        <v>184</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>126</v>
+        <v>185</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>150</v>
+        <v>187</v>
       </c>
       <c r="E33" s="2">
         <v>30</v>
@@ -2520,16 +2594,16 @@
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>103</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>132</v>
+        <v>149</v>
       </c>
       <c r="E34" s="2">
         <v>30</v>
@@ -2537,18 +2611,69 @@
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>104</v>
       </c>
       <c r="D35" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="E35" s="2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="E36" s="2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="E37" s="2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D38" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="E35" s="2">
+      <c r="E38" s="2">
         <v>30</v>
       </c>
     </row>

</xml_diff>